<commit_message>
Add missing fields in import feature.
</commit_message>
<xml_diff>
--- a/src/public/templates/template.xlsx
+++ b/src/public/templates/template.xlsx
@@ -397,7 +397,213 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Numérique
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Valeur entière
+Peux être vide</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Numérique
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Valeur entière
+Peux être vide</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Enumération
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Valeurs possibles :
+- Oui
+- Non</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Enumération
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Valeurs possibles :
+- Oui
+- Non</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Enumération
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Valeurs possibles :
+- Oui
+- Non</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Enumération
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Valeurs possibles :
+- Oui
+- Non</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Enumération
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Valeurs possibles :
+- Oui
+- Non</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Enumération
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Valeurs possibles :
+- Oui
+- Non</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -420,7 +626,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -443,7 +649,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="X1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -466,7 +672,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -489,7 +695,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="Z1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -512,7 +718,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="AA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -535,7 +741,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1">
+    <comment ref="AB1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -582,7 +788,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1">
+    <comment ref="AC1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -655,7 +861,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1">
+    <comment ref="AD1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -685,7 +891,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Nom</t>
   </si>
@@ -751,13 +957,37 @@
   </si>
   <si>
     <t>Secteurs</t>
+  </si>
+  <si>
+    <t>Surface Vente (to)</t>
+  </si>
+  <si>
+    <t>Surface Vente (from)</t>
+  </si>
+  <si>
+    <t>Extraction</t>
+  </si>
+  <si>
+    <t>Appartement</t>
+  </si>
+  <si>
+    <t>License II</t>
+  </si>
+  <si>
+    <t>License III</t>
+  </si>
+  <si>
+    <t>License IV</t>
+  </si>
+  <si>
+    <t>Terrasse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -827,6 +1057,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -862,13 +1099,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:V12" totalsRowShown="0">
-  <autoFilter ref="A1:V12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:AD12" totalsRowShown="0">
+  <autoFilter ref="A1:AD12">
+    <filterColumn colId="13"/>
+    <filterColumn colId="14"/>
+    <filterColumn colId="15"/>
+    <filterColumn colId="16"/>
+    <filterColumn colId="17"/>
+    <filterColumn colId="18"/>
     <filterColumn colId="19"/>
     <filterColumn colId="20"/>
-    <filterColumn colId="21"/>
+    <filterColumn colId="27"/>
+    <filterColumn colId="28"/>
+    <filterColumn colId="29"/>
   </autoFilter>
-  <tableColumns count="22">
+  <tableColumns count="30">
     <tableColumn id="1" name="Nom"/>
     <tableColumn id="2" name="Prénom"/>
     <tableColumn id="3" name="Téléphone"/>
@@ -882,6 +1127,14 @@
     <tableColumn id="11" name="Loyer (to)"/>
     <tableColumn id="12" name="Surface (from)"/>
     <tableColumn id="13" name="Surface (to)"/>
+    <tableColumn id="24" name="Surface Vente (from)"/>
+    <tableColumn id="20" name="Surface Vente (to)"/>
+    <tableColumn id="30" name="Terrasse"/>
+    <tableColumn id="29" name="Extraction"/>
+    <tableColumn id="28" name="Appartement"/>
+    <tableColumn id="27" name="License II"/>
+    <tableColumn id="26" name="License III"/>
+    <tableColumn id="25" name="License IV"/>
     <tableColumn id="14" name="Société"/>
     <tableColumn id="15" name="Mandat"/>
     <tableColumn id="16" name="Adresse (numéro)"/>
@@ -1181,7 +1434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:AD12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1202,18 +1455,26 @@
     <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="1025" width="11.54296875"/>
+    <col min="14" max="14" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="1033" width="11.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1254,34 +1515,58 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="W1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="X1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Y1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Z1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AA1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AB1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AC1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AD1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:30">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1301,8 +1586,16 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:30">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1322,6 +1615,14 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>